<commit_message>
senescence doy 245 missing 3 species in b1
</commit_message>
<xml_diff>
--- a/data/monitoringPhenology/2025-245_Senescence.xlsx
+++ b/data/monitoringPhenology/2025-245_Senescence.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/github/fuelinex/data/monitoringPhenology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2505690E-1D78-084E-85DE-5930050361D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58100F3D-AE8B-3644-B49D-533DEB015AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="shoot_elongation" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">shoot_elongation!$D$1:$D$437</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">shoot_elongation!$D$1:$D$435</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1776" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1760" uniqueCount="467">
   <si>
     <t>tree_ID</t>
   </si>
@@ -1274,9 +1274,6 @@
     <t>Quma_CoolS/WarmF_B3_R13</t>
   </si>
   <si>
-    <t>Quma_CoolS/WarmF_B3_R14</t>
-  </si>
-  <si>
     <t>Quma_CoolS/WarmF_B3_R15</t>
   </si>
   <si>
@@ -1338,9 +1335,6 @@
   </si>
   <si>
     <t>Quma_WarmS/WarmF_B1_R5</t>
-  </si>
-  <si>
-    <t>Quma_WarmS/WarmF_B2_R6</t>
   </si>
   <si>
     <t>Quma_WarmS/WarmF_B2_R7</t>
@@ -2300,8 +2294,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{427BC000-52E3-6840-B950-CDCA9CA72D7D}" name="Table1" displayName="Table1" ref="A1:M437" totalsRowShown="0" dataDxfId="13">
-  <autoFilter ref="A1:M437" xr:uid="{427BC000-52E3-6840-B950-CDCA9CA72D7D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{427BC000-52E3-6840-B950-CDCA9CA72D7D}" name="Table1" displayName="Table1" ref="A1:M435" totalsRowShown="0" dataDxfId="13">
+  <autoFilter ref="A1:M435" xr:uid="{427BC000-52E3-6840-B950-CDCA9CA72D7D}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{0515CFC8-9FED-CA41-BC7E-0EADE3E17C0D}" name="tree_ID" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{C257128B-E55F-4840-ABD4-C2DA6F8965CA}" name="bloc" dataDxfId="11"/>
@@ -2638,12 +2632,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M437"/>
+  <dimension ref="A1:M435"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="185" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="185" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A493" sqref="A493"/>
-      <selection pane="topRight" activeCell="G10" sqref="G10"/>
+      <selection pane="topRight" activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2675,25 +2669,25 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>456</v>
+      </c>
+      <c r="H1" t="s">
+        <v>457</v>
+      </c>
+      <c r="I1" t="s">
         <v>458</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>459</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>460</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>461</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>462</v>
-      </c>
-      <c r="L1" t="s">
-        <v>463</v>
-      </c>
-      <c r="M1" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -2873,7 +2867,7 @@
         <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="G7">
         <v>245</v>
@@ -3324,7 +3318,7 @@
         <v>9</v>
       </c>
       <c r="F21" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="G21">
         <v>245</v>
@@ -4319,7 +4313,7 @@
         <v>9</v>
       </c>
       <c r="F52" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="G52">
         <v>245</v>
@@ -4866,7 +4860,7 @@
         <v>9</v>
       </c>
       <c r="F69" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="G69">
         <v>245</v>
@@ -11397,7 +11391,7 @@
         <v>286</v>
       </c>
       <c r="F273" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="G273">
         <v>245</v>
@@ -13608,7 +13602,7 @@
         <v>286</v>
       </c>
       <c r="F342" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="G342">
         <v>245</v>
@@ -13870,22 +13864,22 @@
         <v>245</v>
       </c>
       <c r="H350" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="I350" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="J350" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="K350">
         <v>0</v>
       </c>
       <c r="L350" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="M350" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="351" spans="1:13" x14ac:dyDescent="0.2">
@@ -15187,17 +15181,17 @@
       <c r="G391">
         <v>245</v>
       </c>
-      <c r="H391" t="s">
-        <v>468</v>
-      </c>
-      <c r="I391" t="s">
-        <v>468</v>
-      </c>
-      <c r="J391" t="s">
-        <v>468</v>
-      </c>
-      <c r="K391" t="s">
-        <v>468</v>
+      <c r="H391">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="I391">
+        <v>17.3</v>
+      </c>
+      <c r="J391">
+        <v>7.7</v>
+      </c>
+      <c r="K391">
+        <v>70</v>
       </c>
     </row>
     <row r="392" spans="1:11" x14ac:dyDescent="0.2">
@@ -15205,10 +15199,10 @@
         <v>412</v>
       </c>
       <c r="B392">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C392" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="D392" t="s">
         <v>367</v>
@@ -15220,13 +15214,13 @@
         <v>245</v>
       </c>
       <c r="H392">
-        <v>9.3000000000000007</v>
+        <v>10</v>
       </c>
       <c r="I392">
-        <v>17.3</v>
+        <v>16.7</v>
       </c>
       <c r="J392">
-        <v>7.7</v>
+        <v>13.6</v>
       </c>
       <c r="K392">
         <v>70</v>
@@ -15252,16 +15246,16 @@
         <v>245</v>
       </c>
       <c r="H393">
-        <v>10</v>
+        <v>13.3</v>
       </c>
       <c r="I393">
-        <v>16.7</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="J393">
-        <v>13.6</v>
+        <v>11.4</v>
       </c>
       <c r="K393">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="394" spans="1:11" x14ac:dyDescent="0.2">
@@ -15284,13 +15278,13 @@
         <v>245</v>
       </c>
       <c r="H394">
-        <v>13.3</v>
+        <v>11.4</v>
       </c>
       <c r="I394">
-        <v>16.100000000000001</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="J394">
-        <v>11.4</v>
+        <v>12</v>
       </c>
       <c r="K394">
         <v>80</v>
@@ -15316,16 +15310,16 @@
         <v>245</v>
       </c>
       <c r="H395">
-        <v>11.4</v>
+        <v>12</v>
       </c>
       <c r="I395">
-        <v>8.3000000000000007</v>
+        <v>12.4</v>
       </c>
       <c r="J395">
-        <v>12</v>
+        <v>8.6</v>
       </c>
       <c r="K395">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="396" spans="1:11" x14ac:dyDescent="0.2">
@@ -15348,16 +15342,16 @@
         <v>245</v>
       </c>
       <c r="H396">
+        <v>7.6</v>
+      </c>
+      <c r="I396">
+        <v>13.9</v>
+      </c>
+      <c r="J396">
         <v>12</v>
       </c>
-      <c r="I396">
-        <v>12.4</v>
-      </c>
-      <c r="J396">
-        <v>8.6</v>
-      </c>
       <c r="K396">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="397" spans="1:11" x14ac:dyDescent="0.2">
@@ -15365,7 +15359,7 @@
         <v>417</v>
       </c>
       <c r="B397">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C397" t="s">
         <v>57</v>
@@ -15380,16 +15374,16 @@
         <v>245</v>
       </c>
       <c r="H397">
-        <v>7.6</v>
+        <v>15.2</v>
       </c>
       <c r="I397">
-        <v>13.9</v>
+        <v>21.4</v>
       </c>
       <c r="J397">
-        <v>12</v>
+        <v>21.6</v>
       </c>
       <c r="K397">
-        <v>70</v>
+        <v>90</v>
       </c>
     </row>
     <row r="398" spans="1:11" x14ac:dyDescent="0.2">
@@ -15412,16 +15406,16 @@
         <v>245</v>
       </c>
       <c r="H398">
-        <v>15.2</v>
+        <v>13.4</v>
       </c>
       <c r="I398">
-        <v>21.4</v>
+        <v>16.5</v>
       </c>
       <c r="J398">
-        <v>21.6</v>
+        <v>15.7</v>
       </c>
       <c r="K398">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="399" spans="1:11" x14ac:dyDescent="0.2">
@@ -15444,16 +15438,16 @@
         <v>245</v>
       </c>
       <c r="H399">
-        <v>13.4</v>
+        <v>9.9</v>
       </c>
       <c r="I399">
-        <v>16.5</v>
+        <v>6.2</v>
       </c>
       <c r="J399">
-        <v>15.7</v>
+        <v>8.5</v>
       </c>
       <c r="K399">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="400" spans="1:11" x14ac:dyDescent="0.2">
@@ -15476,13 +15470,13 @@
         <v>245</v>
       </c>
       <c r="H400">
-        <v>9.9</v>
+        <v>21.3</v>
       </c>
       <c r="I400">
-        <v>6.2</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="J400">
-        <v>8.5</v>
+        <v>21.3</v>
       </c>
       <c r="K400">
         <v>70</v>
@@ -15508,16 +15502,16 @@
         <v>245</v>
       </c>
       <c r="H401">
-        <v>21.3</v>
+        <v>20.2</v>
       </c>
       <c r="I401">
-        <v>16.899999999999999</v>
+        <v>23.6</v>
       </c>
       <c r="J401">
-        <v>21.3</v>
+        <v>26.1</v>
       </c>
       <c r="K401">
-        <v>70</v>
+        <v>95</v>
       </c>
     </row>
     <row r="402" spans="1:11" x14ac:dyDescent="0.2">
@@ -15525,7 +15519,7 @@
         <v>422</v>
       </c>
       <c r="B402">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C402" t="s">
         <v>57</v>
@@ -15540,16 +15534,16 @@
         <v>245</v>
       </c>
       <c r="H402">
-        <v>20.2</v>
+        <v>27.1</v>
       </c>
       <c r="I402">
-        <v>23.6</v>
+        <v>28.2</v>
       </c>
       <c r="J402">
-        <v>26.1</v>
+        <v>31.1</v>
       </c>
       <c r="K402">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="403" spans="1:11" x14ac:dyDescent="0.2">
@@ -15572,16 +15566,16 @@
         <v>245</v>
       </c>
       <c r="H403">
-        <v>27.1</v>
+        <v>24.1</v>
       </c>
       <c r="I403">
-        <v>28.2</v>
+        <v>29.9</v>
       </c>
       <c r="J403">
-        <v>31.1</v>
+        <v>21</v>
       </c>
       <c r="K403">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="404" spans="1:11" x14ac:dyDescent="0.2">
@@ -15604,16 +15598,16 @@
         <v>245</v>
       </c>
       <c r="H404">
-        <v>24.1</v>
+        <v>27.9</v>
       </c>
       <c r="I404">
-        <v>29.9</v>
+        <v>29.4</v>
       </c>
       <c r="J404">
-        <v>21</v>
+        <v>29.1</v>
       </c>
       <c r="K404">
-        <v>80</v>
+        <v>95</v>
       </c>
     </row>
     <row r="405" spans="1:11" x14ac:dyDescent="0.2">
@@ -15636,16 +15630,16 @@
         <v>245</v>
       </c>
       <c r="H405">
-        <v>27.9</v>
+        <v>30</v>
       </c>
       <c r="I405">
-        <v>29.4</v>
+        <v>26.9</v>
       </c>
       <c r="J405">
-        <v>29.1</v>
+        <v>22.6</v>
       </c>
       <c r="K405">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="406" spans="1:11" x14ac:dyDescent="0.2">
@@ -15668,13 +15662,13 @@
         <v>245</v>
       </c>
       <c r="H406">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I406">
-        <v>26.9</v>
+        <v>27.8</v>
       </c>
       <c r="J406">
-        <v>22.6</v>
+        <v>22.4</v>
       </c>
       <c r="K406">
         <v>90</v>
@@ -15685,10 +15679,10 @@
         <v>427</v>
       </c>
       <c r="B407">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C407" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="D407" t="s">
         <v>367</v>
@@ -15700,16 +15694,16 @@
         <v>245</v>
       </c>
       <c r="H407">
-        <v>31</v>
+        <v>14.8</v>
       </c>
       <c r="I407">
-        <v>27.8</v>
+        <v>12.1</v>
       </c>
       <c r="J407">
-        <v>22.4</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="K407">
-        <v>90</v>
+        <v>70</v>
       </c>
     </row>
     <row r="408" spans="1:11" x14ac:dyDescent="0.2">
@@ -15732,16 +15726,16 @@
         <v>245</v>
       </c>
       <c r="H408">
-        <v>14.8</v>
+        <v>8</v>
       </c>
       <c r="I408">
-        <v>12.1</v>
+        <v>10.9</v>
       </c>
       <c r="J408">
-        <v>19.899999999999999</v>
+        <v>12.4</v>
       </c>
       <c r="K408">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="409" spans="1:11" x14ac:dyDescent="0.2">
@@ -15764,13 +15758,13 @@
         <v>245</v>
       </c>
       <c r="H409">
-        <v>8</v>
+        <v>13.3</v>
       </c>
       <c r="I409">
-        <v>10.9</v>
+        <v>15.9</v>
       </c>
       <c r="J409">
-        <v>12.4</v>
+        <v>12.2</v>
       </c>
       <c r="K409">
         <v>80</v>
@@ -15796,16 +15790,16 @@
         <v>245</v>
       </c>
       <c r="H410">
-        <v>13.3</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="I410">
-        <v>15.9</v>
+        <v>11.6</v>
       </c>
       <c r="J410">
-        <v>12.2</v>
+        <v>13.2</v>
       </c>
       <c r="K410">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="411" spans="1:11" x14ac:dyDescent="0.2">
@@ -15828,16 +15822,16 @@
         <v>245</v>
       </c>
       <c r="H411">
-        <v>9.8000000000000007</v>
+        <v>6.1</v>
       </c>
       <c r="I411">
-        <v>11.6</v>
+        <v>6.2</v>
       </c>
       <c r="J411">
-        <v>13.2</v>
+        <v>7.1</v>
       </c>
       <c r="K411">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="412" spans="1:11" x14ac:dyDescent="0.2">
@@ -15845,7 +15839,7 @@
         <v>432</v>
       </c>
       <c r="B412">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C412" t="s">
         <v>73</v>
@@ -15860,16 +15854,16 @@
         <v>245</v>
       </c>
       <c r="H412">
-        <v>6.1</v>
+        <v>20.8</v>
       </c>
       <c r="I412">
-        <v>6.2</v>
+        <v>24.4</v>
       </c>
       <c r="J412">
-        <v>7.1</v>
+        <v>22.4</v>
       </c>
       <c r="K412">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="413" spans="1:11" x14ac:dyDescent="0.2">
@@ -15891,17 +15885,17 @@
       <c r="G413">
         <v>245</v>
       </c>
-      <c r="H413" t="s">
-        <v>468</v>
-      </c>
-      <c r="I413" t="s">
-        <v>468</v>
-      </c>
-      <c r="J413" t="s">
-        <v>468</v>
-      </c>
-      <c r="K413" t="s">
-        <v>468</v>
+      <c r="H413">
+        <v>13.6</v>
+      </c>
+      <c r="I413">
+        <v>11.9</v>
+      </c>
+      <c r="J413">
+        <v>8.6</v>
+      </c>
+      <c r="K413">
+        <v>70</v>
       </c>
     </row>
     <row r="414" spans="1:11" x14ac:dyDescent="0.2">
@@ -15924,13 +15918,13 @@
         <v>245</v>
       </c>
       <c r="H414">
-        <v>20.8</v>
+        <v>17</v>
       </c>
       <c r="I414">
-        <v>24.4</v>
+        <v>18.2</v>
       </c>
       <c r="J414">
-        <v>22.4</v>
+        <v>23.1</v>
       </c>
       <c r="K414">
         <v>80</v>
@@ -15956,16 +15950,16 @@
         <v>245</v>
       </c>
       <c r="H415">
-        <v>13.6</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="I415">
-        <v>11.9</v>
+        <v>21.9</v>
       </c>
       <c r="J415">
-        <v>8.6</v>
+        <v>20.5</v>
       </c>
       <c r="K415">
-        <v>70</v>
+        <v>90</v>
       </c>
     </row>
     <row r="416" spans="1:11" x14ac:dyDescent="0.2">
@@ -15973,7 +15967,7 @@
         <v>436</v>
       </c>
       <c r="B416">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C416" t="s">
         <v>73</v>
@@ -15988,16 +15982,16 @@
         <v>245</v>
       </c>
       <c r="H416">
-        <v>17</v>
+        <v>30.7</v>
       </c>
       <c r="I416">
-        <v>18.2</v>
+        <v>21.5</v>
       </c>
       <c r="J416">
-        <v>23.1</v>
+        <v>24</v>
       </c>
       <c r="K416">
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="417" spans="1:11" x14ac:dyDescent="0.2">
@@ -16005,7 +15999,7 @@
         <v>437</v>
       </c>
       <c r="B417">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C417" t="s">
         <v>73</v>
@@ -16020,16 +16014,16 @@
         <v>245</v>
       </c>
       <c r="H417">
-        <v>16.100000000000001</v>
+        <v>12.5</v>
       </c>
       <c r="I417">
-        <v>21.9</v>
+        <v>13.9</v>
       </c>
       <c r="J417">
-        <v>20.5</v>
+        <v>21.1</v>
       </c>
       <c r="K417">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="418" spans="1:11" x14ac:dyDescent="0.2">
@@ -16052,16 +16046,16 @@
         <v>245</v>
       </c>
       <c r="H418">
-        <v>30.7</v>
+        <v>14.6</v>
       </c>
       <c r="I418">
-        <v>21.5</v>
+        <v>12</v>
       </c>
       <c r="J418">
-        <v>24</v>
+        <v>12.2</v>
       </c>
       <c r="K418">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="419" spans="1:11" x14ac:dyDescent="0.2">
@@ -16084,13 +16078,13 @@
         <v>245</v>
       </c>
       <c r="H419">
-        <v>12.5</v>
+        <v>23</v>
       </c>
       <c r="I419">
-        <v>13.9</v>
+        <v>19.7</v>
       </c>
       <c r="J419">
-        <v>21.1</v>
+        <v>32.4</v>
       </c>
       <c r="K419">
         <v>80</v>
@@ -16116,13 +16110,13 @@
         <v>245</v>
       </c>
       <c r="H420">
-        <v>14.6</v>
+        <v>18.8</v>
       </c>
       <c r="I420">
-        <v>12</v>
+        <v>19.8</v>
       </c>
       <c r="J420">
-        <v>12.2</v>
+        <v>27.4</v>
       </c>
       <c r="K420">
         <v>80</v>
@@ -16133,10 +16127,10 @@
         <v>441</v>
       </c>
       <c r="B421">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C421" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="D421" t="s">
         <v>367</v>
@@ -16148,16 +16142,16 @@
         <v>245</v>
       </c>
       <c r="H421">
-        <v>23</v>
+        <v>13.5</v>
       </c>
       <c r="I421">
-        <v>19.7</v>
+        <v>16.5</v>
       </c>
       <c r="J421">
-        <v>32.4</v>
+        <v>11.9</v>
       </c>
       <c r="K421">
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="422" spans="1:11" x14ac:dyDescent="0.2">
@@ -16165,10 +16159,10 @@
         <v>442</v>
       </c>
       <c r="B422">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C422" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="D422" t="s">
         <v>367</v>
@@ -16180,16 +16174,16 @@
         <v>245</v>
       </c>
       <c r="H422">
-        <v>18.8</v>
+        <v>14.8</v>
       </c>
       <c r="I422">
-        <v>19.8</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="J422">
-        <v>27.4</v>
+        <v>17.3</v>
       </c>
       <c r="K422">
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="423" spans="1:11" x14ac:dyDescent="0.2">
@@ -16212,16 +16206,16 @@
         <v>245</v>
       </c>
       <c r="H423">
+        <v>15.7</v>
+      </c>
+      <c r="I423">
+        <v>22.3</v>
+      </c>
+      <c r="J423">
         <v>13.5</v>
       </c>
-      <c r="I423">
-        <v>16.5</v>
-      </c>
-      <c r="J423">
-        <v>11.9</v>
-      </c>
       <c r="K423">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="424" spans="1:11" x14ac:dyDescent="0.2">
@@ -16244,16 +16238,16 @@
         <v>245</v>
       </c>
       <c r="H424">
-        <v>14.8</v>
+        <v>16.2</v>
       </c>
       <c r="I424">
-        <v>19.100000000000001</v>
+        <v>17.8</v>
       </c>
       <c r="J424">
-        <v>17.3</v>
+        <v>16.2</v>
       </c>
       <c r="K424">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="425" spans="1:11" x14ac:dyDescent="0.2">
@@ -16276,16 +16270,16 @@
         <v>245</v>
       </c>
       <c r="H425">
-        <v>15.7</v>
+        <v>11.3</v>
       </c>
       <c r="I425">
-        <v>22.3</v>
+        <v>10</v>
       </c>
       <c r="J425">
-        <v>13.5</v>
+        <v>9.9</v>
       </c>
       <c r="K425">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="426" spans="1:11" x14ac:dyDescent="0.2">
@@ -16293,7 +16287,7 @@
         <v>446</v>
       </c>
       <c r="B426">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C426" t="s">
         <v>89</v>
@@ -16308,16 +16302,16 @@
         <v>245</v>
       </c>
       <c r="H426">
-        <v>16.2</v>
+        <v>24.1</v>
       </c>
       <c r="I426">
-        <v>17.8</v>
+        <v>24.2</v>
       </c>
       <c r="J426">
-        <v>16.2</v>
+        <v>21.3</v>
       </c>
       <c r="K426">
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="427" spans="1:11" x14ac:dyDescent="0.2">
@@ -16325,7 +16319,7 @@
         <v>447</v>
       </c>
       <c r="B427">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C427" t="s">
         <v>89</v>
@@ -16340,16 +16334,16 @@
         <v>245</v>
       </c>
       <c r="H427">
-        <v>11.3</v>
+        <v>8.6</v>
       </c>
       <c r="I427">
-        <v>10</v>
+        <v>9.4</v>
       </c>
       <c r="J427">
-        <v>9.9</v>
+        <v>11</v>
       </c>
       <c r="K427">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="428" spans="1:11" x14ac:dyDescent="0.2">
@@ -16372,16 +16366,16 @@
         <v>245</v>
       </c>
       <c r="H428">
-        <v>24.1</v>
+        <v>7</v>
       </c>
       <c r="I428">
-        <v>24.2</v>
+        <v>6.8</v>
       </c>
       <c r="J428">
-        <v>21.3</v>
+        <v>8.4</v>
       </c>
       <c r="K428">
-        <v>90</v>
+        <v>60</v>
       </c>
     </row>
     <row r="429" spans="1:11" x14ac:dyDescent="0.2">
@@ -16404,13 +16398,13 @@
         <v>245</v>
       </c>
       <c r="H429">
-        <v>8.6</v>
+        <v>11.1</v>
       </c>
       <c r="I429">
-        <v>9.4</v>
+        <v>12.4</v>
       </c>
       <c r="J429">
-        <v>11</v>
+        <v>10.6</v>
       </c>
       <c r="K429">
         <v>70</v>
@@ -16436,16 +16430,16 @@
         <v>245</v>
       </c>
       <c r="H430">
-        <v>7</v>
+        <v>13.6</v>
       </c>
       <c r="I430">
-        <v>6.8</v>
+        <v>20.9</v>
       </c>
       <c r="J430">
-        <v>8.4</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="K430">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="431" spans="1:11" x14ac:dyDescent="0.2">
@@ -16453,7 +16447,7 @@
         <v>451</v>
       </c>
       <c r="B431">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C431" t="s">
         <v>89</v>
@@ -16468,16 +16462,16 @@
         <v>245</v>
       </c>
       <c r="H431">
-        <v>11.1</v>
+        <v>30.7</v>
       </c>
       <c r="I431">
-        <v>12.4</v>
+        <v>32.1</v>
       </c>
       <c r="J431">
-        <v>10.6</v>
+        <v>29.9</v>
       </c>
       <c r="K431">
-        <v>70</v>
+        <v>90</v>
       </c>
     </row>
     <row r="432" spans="1:11" x14ac:dyDescent="0.2">
@@ -16485,7 +16479,7 @@
         <v>452</v>
       </c>
       <c r="B432">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C432" t="s">
         <v>89</v>
@@ -16500,13 +16494,13 @@
         <v>245</v>
       </c>
       <c r="H432">
-        <v>13.6</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="I432">
-        <v>20.9</v>
+        <v>15.1</v>
       </c>
       <c r="J432">
-        <v>17.600000000000001</v>
+        <v>16.5</v>
       </c>
       <c r="K432">
         <v>80</v>
@@ -16532,16 +16526,16 @@
         <v>245</v>
       </c>
       <c r="H433">
-        <v>30.7</v>
+        <v>19.3</v>
       </c>
       <c r="I433">
-        <v>32.1</v>
+        <v>13.6</v>
       </c>
       <c r="J433">
-        <v>29.9</v>
+        <v>12.9</v>
       </c>
       <c r="K433">
-        <v>90</v>
+        <v>70</v>
       </c>
     </row>
     <row r="434" spans="1:11" x14ac:dyDescent="0.2">
@@ -16564,13 +16558,13 @@
         <v>245</v>
       </c>
       <c r="H434">
-        <v>19.899999999999999</v>
+        <v>25.1</v>
       </c>
       <c r="I434">
-        <v>15.1</v>
+        <v>23.5</v>
       </c>
       <c r="J434">
-        <v>16.5</v>
+        <v>19.5</v>
       </c>
       <c r="K434">
         <v>80</v>
@@ -16596,79 +16590,15 @@
         <v>245</v>
       </c>
       <c r="H435">
-        <v>19.3</v>
+        <v>21.3</v>
       </c>
       <c r="I435">
-        <v>13.6</v>
+        <v>22.7</v>
       </c>
       <c r="J435">
-        <v>12.9</v>
+        <v>22.6</v>
       </c>
       <c r="K435">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="436" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A436" t="s">
-        <v>456</v>
-      </c>
-      <c r="B436">
-        <v>3</v>
-      </c>
-      <c r="C436" t="s">
-        <v>89</v>
-      </c>
-      <c r="D436" t="s">
-        <v>367</v>
-      </c>
-      <c r="E436" t="s">
-        <v>368</v>
-      </c>
-      <c r="G436">
-        <v>245</v>
-      </c>
-      <c r="H436">
-        <v>25.1</v>
-      </c>
-      <c r="I436">
-        <v>23.5</v>
-      </c>
-      <c r="J436">
-        <v>19.5</v>
-      </c>
-      <c r="K436">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="437" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A437" t="s">
-        <v>457</v>
-      </c>
-      <c r="B437">
-        <v>3</v>
-      </c>
-      <c r="C437" t="s">
-        <v>89</v>
-      </c>
-      <c r="D437" t="s">
-        <v>367</v>
-      </c>
-      <c r="E437" t="s">
-        <v>368</v>
-      </c>
-      <c r="G437">
-        <v>245</v>
-      </c>
-      <c r="H437">
-        <v>21.3</v>
-      </c>
-      <c r="I437">
-        <v>22.7</v>
-      </c>
-      <c r="J437">
-        <v>22.6</v>
-      </c>
-      <c r="K437">
         <v>80</v>
       </c>
     </row>

</xml_diff>